<commit_message>
Updated comments structure and added venv
</commit_message>
<xml_diff>
--- a/11000.xlsx
+++ b/11000.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zkoqm/Desktop/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7113161-5D94-6345-8FE3-2497D0C9836C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FF5822-6249-8946-A97C-9F78E1502AA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{B24B9D77-B903-7C4B-B678-12FC0ADDB7B9}"/>
   </bookViews>
   <sheets>
     <sheet name="11000" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>